<commit_message>
Database models, view stubs
</commit_message>
<xml_diff>
--- a/docs/Web API.xlsx
+++ b/docs/Web API.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\dev\AMDSS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35ABE8E1-6C9A-49F4-A2D7-58CBBA294983}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A068727-F749-4DE5-813D-FC09595F0D4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{87C8A326-C7AB-4A18-A6BA-C7FA50E30E71}"/>
   </bookViews>
@@ -436,7 +436,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>